<commit_message>
Modified definitions and codded them in
Instead of crossing the cell the right and bottom border are used
</commit_message>
<xml_diff>
--- a/TableFormat_ConversionDefinition.xlsx
+++ b/TableFormat_ConversionDefinition.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C70DB39-CA4A-4E54-B611-EF1690BE2CB9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7235E6-6DEC-472A-9FF3-13DC0504E39C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -299,76 +299,76 @@
     <t>may be added later</t>
   </si>
   <si>
-    <t>crossed \ #????00</t>
-  </si>
-  <si>
-    <t>crossed \ #????55</t>
-  </si>
-  <si>
-    <t>crossed \ #????aa</t>
-  </si>
-  <si>
-    <t>crossed \ #????ff</t>
-  </si>
-  <si>
-    <t>crossed \ #??00??</t>
-  </si>
-  <si>
-    <t>crossed \ #??55??</t>
-  </si>
-  <si>
-    <t>crossed \ #??aa??</t>
-  </si>
-  <si>
-    <t>crossed \ #??ff??</t>
-  </si>
-  <si>
-    <t>crossed \ #00????</t>
-  </si>
-  <si>
-    <t>crossed \ #55????</t>
-  </si>
-  <si>
-    <t>crossed \ #aa????</t>
-  </si>
-  <si>
-    <t>crossed \ #ff????</t>
-  </si>
-  <si>
-    <t>crossed / #????00</t>
-  </si>
-  <si>
-    <t>crossed / #????55</t>
-  </si>
-  <si>
-    <t>crossed / #????aa</t>
-  </si>
-  <si>
-    <t>crossed / #????ff</t>
-  </si>
-  <si>
-    <t>crossed / #??00??</t>
-  </si>
-  <si>
-    <t>crossed / #??55??</t>
-  </si>
-  <si>
-    <t>crossed / #??aa??</t>
-  </si>
-  <si>
-    <t>crossed / #??ff??</t>
-  </si>
-  <si>
-    <t>crossed / #00????</t>
-  </si>
-  <si>
-    <t>crossed / #55????</t>
-  </si>
-  <si>
-    <t>crossed / #aa????</t>
-  </si>
-  <si>
-    <t>crossed / #ff????</t>
+    <t>underlined #????00</t>
+  </si>
+  <si>
+    <t>underlined #????55</t>
+  </si>
+  <si>
+    <t>underlined #????aa</t>
+  </si>
+  <si>
+    <t>underlined #????ff</t>
+  </si>
+  <si>
+    <t>underlined #??00??</t>
+  </si>
+  <si>
+    <t>underlined #??55??</t>
+  </si>
+  <si>
+    <t>underlined #??aa??</t>
+  </si>
+  <si>
+    <t>underlined #??ff??</t>
+  </si>
+  <si>
+    <t>underlined #00????</t>
+  </si>
+  <si>
+    <t>underlined #55????</t>
+  </si>
+  <si>
+    <t>underlined #aa????</t>
+  </si>
+  <si>
+    <t>underlined #ff????</t>
+  </si>
+  <si>
+    <t>right border #????00</t>
+  </si>
+  <si>
+    <t>right border #????55</t>
+  </si>
+  <si>
+    <t>right border #????aa</t>
+  </si>
+  <si>
+    <t>right border #????ff</t>
+  </si>
+  <si>
+    <t>right border #??00??</t>
+  </si>
+  <si>
+    <t>right border #??55??</t>
+  </si>
+  <si>
+    <t>right border #??aa??</t>
+  </si>
+  <si>
+    <t>right border #??ff??</t>
+  </si>
+  <si>
+    <t>right border #00????</t>
+  </si>
+  <si>
+    <t>right border #55????</t>
+  </si>
+  <si>
+    <t>right border #aa????</t>
+  </si>
+  <si>
+    <t>right border #ff????</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -530,191 +530,231 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="1">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal style="thin">
+      <bottom style="thin">
         <color rgb="FFFFFF00"/>
-      </diagonal>
+      </bottom>
+      <diagonal/>
     </border>
-    <border diagonalUp="1">
+    <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color rgb="FFFFFF00"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFF55"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFFFF55"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFFFFAA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFF00"/>
+      </right>
       <top/>
       <bottom/>
-      <diagonal style="thin">
-        <color rgb="FFFFFF00"/>
-      </diagonal>
+      <diagonal/>
     </border>
-    <border diagonalDown="1">
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFF55"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFAA"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF00FF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF55FF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFAAFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF00FFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF55FFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFAAFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FFFFFF55"/>
-      </diagonal>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF00FF"/>
+      </bottom>
+      <diagonal/>
     </border>
-    <border diagonalUp="1">
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FFFFFF55"/>
-      </diagonal>
+      <top style="thin">
+        <color rgb="FFFF00FF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF55FF"/>
+      </bottom>
+      <diagonal/>
     </border>
-    <border diagonalDown="1">
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FFFFFFAA"/>
-      </diagonal>
+      <top style="thin">
+        <color rgb="FFFF55FF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFAAFF"/>
+      </bottom>
+      <diagonal/>
     </border>
-    <border diagonalUp="1">
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FFFFFFAA"/>
-      </diagonal>
+      <top style="thin">
+        <color rgb="FFFFAAFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
     </border>
-    <border diagonalDown="1">
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
+      <top style="thin">
         <color rgb="FFFFFFFF"/>
-      </diagonal>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00FFFF"/>
+      </bottom>
+      <diagonal/>
     </border>
-    <border diagonalUp="1">
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FFFFFFFF"/>
-      </diagonal>
+      <top style="thin">
+        <color rgb="FF00FFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF55FFFF"/>
+      </bottom>
+      <diagonal/>
     </border>
-    <border diagonalDown="1">
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FFFF00FF"/>
-      </diagonal>
+      <top style="thin">
+        <color rgb="FF55FFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFAAFFFF"/>
+      </bottom>
+      <diagonal/>
     </border>
-    <border diagonalUp="1">
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FFFF00FF"/>
-      </diagonal>
-    </border>
-    <border diagonalDown="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FFFF55FF"/>
-      </diagonal>
-    </border>
-    <border diagonalUp="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FFFF55FF"/>
-      </diagonal>
-    </border>
-    <border diagonalDown="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FFFFAAFF"/>
-      </diagonal>
-    </border>
-    <border diagonalUp="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FFFFAAFF"/>
-      </diagonal>
-    </border>
-    <border diagonalDown="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FF00FFFF"/>
-      </diagonal>
-    </border>
-    <border diagonalUp="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FF00FFFF"/>
-      </diagonal>
-    </border>
-    <border diagonalDown="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FF55FFFF"/>
-      </diagonal>
-    </border>
-    <border diagonalUp="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FF55FFFF"/>
-      </diagonal>
-    </border>
-    <border diagonalDown="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
+      <top style="thin">
         <color rgb="FFAAFFFF"/>
-      </diagonal>
-    </border>
-    <border diagonalUp="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color rgb="FFAAFFFF"/>
-      </diagonal>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -758,6 +798,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -771,8 +813,8 @@
       <color rgb="FF55FFFF"/>
       <color rgb="FF00FFFF"/>
       <color rgb="FFFFAAFF"/>
+      <color rgb="FFFF00FF"/>
       <color rgb="FFFF55FF"/>
-      <color rgb="FFFF00FF"/>
       <color rgb="FFFFFFAA"/>
       <color rgb="FFFFFF55"/>
       <color rgb="FFFFFF00"/>
@@ -1054,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28:O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,7 +1630,7 @@
       <c r="A27" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="6">
@@ -1608,7 +1650,7 @@
       <c r="A28" t="s">
         <v>94</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="6">
@@ -1628,7 +1670,7 @@
       <c r="A29" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="6">
@@ -1648,7 +1690,7 @@
       <c r="A30" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="37" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="6">
@@ -1668,7 +1710,7 @@
       <c r="A31" t="s">
         <v>97</v>
       </c>
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="38" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="6">
@@ -1686,7 +1728,7 @@
       <c r="A32" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="39" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="6">
@@ -1704,7 +1746,7 @@
       <c r="A33" t="s">
         <v>99</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="40" t="s">
         <v>3</v>
       </c>
       <c r="C33" s="6">
@@ -1722,7 +1764,7 @@
       <c r="A34" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="41" t="s">
         <v>3</v>
       </c>
       <c r="C34" s="6">
@@ -1740,7 +1782,7 @@
       <c r="A35" t="s">
         <v>101</v>
       </c>
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="42" t="s">
         <v>3</v>
       </c>
       <c r="C35" s="6">
@@ -1758,7 +1800,7 @@
       <c r="A36" t="s">
         <v>102</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="43" t="s">
         <v>3</v>
       </c>
       <c r="C36" s="6">
@@ -1776,7 +1818,7 @@
       <c r="A37" t="s">
         <v>103</v>
       </c>
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="44" t="s">
         <v>3</v>
       </c>
       <c r="C37" s="6">
@@ -1794,7 +1836,7 @@
       <c r="A38" t="s">
         <v>104</v>
       </c>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="27" t="s">
         <v>3</v>
       </c>
       <c r="C38" s="6">
@@ -1812,7 +1854,7 @@
       <c r="A39" t="s">
         <v>105</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="28" t="s">
         <v>3</v>
       </c>
       <c r="C39" s="6">
@@ -1830,7 +1872,7 @@
       <c r="A40" t="s">
         <v>106</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="29" t="s">
         <v>3</v>
       </c>
       <c r="C40" s="6">
@@ -1866,7 +1908,7 @@
       <c r="A42" t="s">
         <v>108</v>
       </c>
-      <c r="B42" s="32" t="s">
+      <c r="B42" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C42" s="6">
@@ -1884,7 +1926,7 @@
       <c r="A43" t="s">
         <v>109</v>
       </c>
-      <c r="B43" s="34" t="s">
+      <c r="B43" s="32" t="s">
         <v>3</v>
       </c>
       <c r="C43" s="6">
@@ -1902,7 +1944,7 @@
       <c r="A44" t="s">
         <v>110</v>
       </c>
-      <c r="B44" s="36" t="s">
+      <c r="B44" s="33" t="s">
         <v>3</v>
       </c>
       <c r="C44" s="6">
@@ -1938,7 +1980,7 @@
       <c r="A46" t="s">
         <v>112</v>
       </c>
-      <c r="B46" s="38" t="s">
+      <c r="B46" s="34" t="s">
         <v>3</v>
       </c>
       <c r="C46" s="6">
@@ -1956,7 +1998,7 @@
       <c r="A47" t="s">
         <v>113</v>
       </c>
-      <c r="B47" s="40" t="s">
+      <c r="B47" s="35" t="s">
         <v>3</v>
       </c>
       <c r="C47" s="6">
@@ -1974,7 +2016,7 @@
       <c r="A48" t="s">
         <v>114</v>
       </c>
-      <c r="B48" s="42" t="s">
+      <c r="B48" s="36" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="6">

</xml_diff>

<commit_message>
Started work on machine
created the EsolangMachine class to act as the machine running the code, some basic components thereof
</commit_message>
<xml_diff>
--- a/TableFormat_ConversionDefinition.xlsx
+++ b/TableFormat_ConversionDefinition.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7235E6-6DEC-472A-9FF3-13DC0504E39C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0921A29C-ECF2-453D-B4A7-5CA56CE18667}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="format to number" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="118">
   <si>
     <t>format description</t>
   </si>
@@ -369,6 +369,12 @@
   </si>
   <si>
     <t>right border #ff????</t>
+  </si>
+  <si>
+    <t>pause</t>
+  </si>
+  <si>
+    <t>for the amount of miliseconds specified by A</t>
   </si>
 </sst>
 </file>
@@ -1096,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28:O31"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2058,8 +2064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F928CD-8A96-42B3-B16E-F8327990D609}">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2489,10 +2495,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="C39" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2500,15 +2506,21 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Big test program work
gonna do something else on this project and want to separate it into a separate commit
</commit_message>
<xml_diff>
--- a/TableFormat_ConversionDefinition.xlsx
+++ b/TableFormat_ConversionDefinition.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED577DF-3495-4980-BB52-A7B9FB4A2C52}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55738340-88E1-454E-A676-EE3EF8E8667F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="format to number" sheetId="1" r:id="rId1"/>
     <sheet name="number to command" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2064,7 +2064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F928CD-8A96-42B3-B16E-F8327990D609}">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>

</xml_diff>